<commit_message>
Implementando TestNG + ExtentReport
</commit_message>
<xml_diff>
--- a/src/main/java/resources/ArquivoExcel.xlsx
+++ b/src/main/java/resources/ArquivoExcel.xlsx
@@ -3,31 +3,29 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{E1AAB701-AA8E-493D-AF8F-7EF483DC55DB}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marcos.souza\Documents\Android\workspace\ProjetoAppiumTDD\src\main\java\resources\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F57306A-8B29-466C-91F8-BFD39E8A9D88}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="15405" windowHeight="11340" xr2:uid="{F2F26E07-A8E5-41D4-BA69-4DBB7253C558}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="15375" windowHeight="7875" xr2:uid="{F2F26E07-A8E5-41D4-BA69-4DBB7253C558}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>e-mail</t>
   </si>
@@ -75,6 +73,12 @@
   </si>
   <si>
     <t>Osasco</t>
+  </si>
+  <si>
+    <t>29827-17</t>
+  </si>
+  <si>
+    <t>11 12121212</t>
   </si>
 </sst>
 </file>
@@ -440,7 +444,7 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -491,8 +495,8 @@
       <c r="D2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E2">
-        <v>1112121212</v>
+      <c r="E2" t="s">
+        <v>17</v>
       </c>
       <c r="F2" t="s">
         <v>13</v>
@@ -503,8 +507,8 @@
       <c r="H2" t="s">
         <v>15</v>
       </c>
-      <c r="I2">
-        <v>2982717</v>
+      <c r="I2" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>